<commit_message>
Commit nuevas caracteristicas II 20-05-2024
</commit_message>
<xml_diff>
--- a/controles_app.xlsx
+++ b/controles_app.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Python QAQC MSB 2\app_contingencia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mahuilque_streamlit\app_contingencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754C98A2-5339-447A-B69A-595D28243C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A165D2-02D5-4920-84A7-6B98ABFEE59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F2D88E9E-A39A-4286-A28D-D176329D37FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F2D88E9E-A39A-4286-A28D-D176329D37FB}"/>
   </bookViews>
   <sheets>
     <sheet name="comportamiento" sheetId="2" r:id="rId1"/>
-    <sheet name="mot_interv" sheetId="4" r:id="rId2"/>
-    <sheet name="area_operativa" sheetId="10" r:id="rId3"/>
-    <sheet name="localidad" sheetId="11" r:id="rId4"/>
-    <sheet name="herpetofauna" sheetId="12" r:id="rId5"/>
-    <sheet name="ornitofauna" sheetId="13" r:id="rId6"/>
-    <sheet name="mastofauna" sheetId="14" r:id="rId7"/>
-    <sheet name="ictiofauna" sheetId="15" r:id="rId8"/>
+    <sheet name="tipo_registro" sheetId="17" r:id="rId2"/>
+    <sheet name="causa_probable" sheetId="16" r:id="rId3"/>
+    <sheet name="mot_interv" sheetId="4" r:id="rId4"/>
+    <sheet name="area_operativa" sheetId="10" r:id="rId5"/>
+    <sheet name="localidad" sheetId="11" r:id="rId6"/>
+    <sheet name="herpetofauna" sheetId="12" r:id="rId7"/>
+    <sheet name="ornitofauna" sheetId="13" r:id="rId8"/>
+    <sheet name="mastofauna" sheetId="14" r:id="rId9"/>
+    <sheet name="ictiofauna" sheetId="15" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="324">
   <si>
     <t>Herpetofauna</t>
   </si>
@@ -940,6 +942,81 @@
   </si>
   <si>
     <t>Bagrecito/Suche</t>
+  </si>
+  <si>
+    <t>causa_probable</t>
+  </si>
+  <si>
+    <t>Atropello</t>
+  </si>
+  <si>
+    <t>Natural</t>
+  </si>
+  <si>
+    <t>Por ataque</t>
+  </si>
+  <si>
+    <t>Ahogado</t>
+  </si>
+  <si>
+    <t>Envenenado</t>
+  </si>
+  <si>
+    <t>Colision</t>
+  </si>
+  <si>
+    <t>Otra causa</t>
+  </si>
+  <si>
+    <t>tipo_registro</t>
+  </si>
+  <si>
+    <t>Auditivo</t>
+  </si>
+  <si>
+    <t>Avistamiento</t>
+  </si>
+  <si>
+    <t>Captura temporal</t>
+  </si>
+  <si>
+    <t>Carcasa/Restos/Osamenta</t>
+  </si>
+  <si>
+    <t>Dormidero</t>
+  </si>
+  <si>
+    <t>Egagropila</t>
+  </si>
+  <si>
+    <t>Estercolero</t>
+  </si>
+  <si>
+    <t>Excavacion</t>
+  </si>
+  <si>
+    <t>Feca</t>
+  </si>
+  <si>
+    <t>Galerias</t>
+  </si>
+  <si>
+    <t>Huella</t>
+  </si>
+  <si>
+    <t>Nido</t>
+  </si>
+  <si>
+    <t>Pelos</t>
+  </si>
+  <si>
+    <t>Piel</t>
+  </si>
+  <si>
+    <t>Plumas</t>
+  </si>
+  <si>
+    <t>Revolcadero</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1082,38 @@
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{93E3A725-0C5A-4812-892E-1AE6BD704C0B}" name="ictiofauna" displayName="ictiofauna" ref="A1:A13" totalsRowShown="0">
+  <autoFilter ref="A1:A13" xr:uid="{93E3A725-0C5A-4812-892E-1AE6BD704C0B}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{8C7BDAF4-0950-472F-BF73-27A1F93B6396}" name="Ictiofauna"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{3AA9C78C-2BA8-44AC-BEC3-4FBA973E6FC5}" name="Tabla10" displayName="Tabla10" ref="A1:B29" totalsRowShown="0">
+  <autoFilter ref="A1:B29" xr:uid="{3AA9C78C-2BA8-44AC-BEC3-4FBA973E6FC5}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{6D795741-B050-430D-8C6A-73ED7B111AE8}" name="tipo_registro"/>
+    <tableColumn id="2" xr3:uid="{BF401F0E-7BA4-4CF3-A76B-8CCA22FF5B14}" name="componente_biologico"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{99AE9F4D-732C-49F9-9BDD-DDF42A1507A7}" name="Tabla4" displayName="Tabla4" ref="A1:A8" totalsRowShown="0">
+  <autoFilter ref="A1:A8" xr:uid="{99AE9F4D-732C-49F9-9BDD-DDF42A1507A7}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{85D336FF-9890-42AA-BF41-1CC4983FA373}" name="causa_probable"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4AD5B25E-FE28-4B3D-AA57-09732E5254D9}" name="mot_interv" displayName="mot_interv" ref="A1:A7" totalsRowShown="0">
   <autoFilter ref="A1:A7" xr:uid="{4AD5B25E-FE28-4B3D-AA57-09732E5254D9}"/>
   <tableColumns count="1">
@@ -1015,7 +1123,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B6C4CE3-EA82-4077-ABF6-27D6E07F483B}" name="aa_oo" displayName="aa_oo" ref="A1:A8" totalsRowShown="0">
   <autoFilter ref="A1:A8" xr:uid="{8B6C4CE3-EA82-4077-ABF6-27D6E07F483B}"/>
   <tableColumns count="1">
@@ -1025,7 +1133,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A94BC538-A411-4E48-9CD7-323BDCDBF047}" name="localidad" displayName="localidad" ref="A1:A16" totalsRowShown="0">
   <autoFilter ref="A1:A16" xr:uid="{A94BC538-A411-4E48-9CD7-323BDCDBF047}"/>
   <tableColumns count="1">
@@ -1035,7 +1143,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4A929AA7-E856-43B9-9AC9-3BE825C19938}" name="herpetofauna" displayName="herpetofauna" ref="A1:A14" totalsRowShown="0">
   <autoFilter ref="A1:A14" xr:uid="{4A929AA7-E856-43B9-9AC9-3BE825C19938}"/>
   <tableColumns count="1">
@@ -1045,7 +1153,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2668E4E0-A4FC-45DA-8A88-3A539497C7BB}" name="ornitofauna" displayName="ornitofauna" ref="A1:A182" totalsRowShown="0">
   <autoFilter ref="A1:A182" xr:uid="{2668E4E0-A4FC-45DA-8A88-3A539497C7BB}"/>
   <tableColumns count="1">
@@ -1055,21 +1163,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{8EE494A1-B267-4FF9-AB06-EDA74775BF2D}" name="mastofauna" displayName="mastofauna" ref="A1:A43" totalsRowShown="0">
   <autoFilter ref="A1:A43" xr:uid="{8EE494A1-B267-4FF9-AB06-EDA74775BF2D}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{45F79B73-A421-4214-83CD-A98D9A476968}" name="Mastofauna"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{93E3A725-0C5A-4812-892E-1AE6BD704C0B}" name="ictiofauna" displayName="ictiofauna" ref="A1:A13" totalsRowShown="0">
-  <autoFilter ref="A1:A13" xr:uid="{93E3A725-0C5A-4812-892E-1AE6BD704C0B}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{8C7BDAF4-0950-472F-BF73-27A1F93B6396}" name="Ictiofauna"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1393,17 +1491,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0845A9DC-B861-4113-8F2B-3F0CB4F28011}">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1749,6 +1847,95 @@
       </c>
       <c r="B43" t="s">
         <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CAE7036-8C5B-4AB4-B879-95C777AB2D1D}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -1760,14 +1947,335 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EA3FD13-8850-4FBC-8EF9-E44C889844C1}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:B29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>310</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>310</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>311</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>311</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>311</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>312</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>312</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>313</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>314</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>315</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>316</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>316</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>316</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>317</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>318</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>318</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>318</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>319</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>320</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>321</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>321</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>322</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>323</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C7C3C8F-9F96-4AE8-96D7-FE49029A6AE0}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>306</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09D83F43-5FA4-4D82-89DC-AC5558E41519}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1819,7 +2327,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B924FBC-C27B-4647-A08C-76C440E03E1E}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -1883,7 +2391,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AEBFB7B-5E7E-47D0-A09F-14DE5718D683}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -1987,7 +2495,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42BBB3F2-2F19-417F-9483-5E65AD0289D5}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -2081,7 +2589,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F986D4-5AA4-4148-9FB2-C51FA9AD084C}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -3015,7 +3523,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A3CFDB-A353-44BC-AB3C-B23FAC2C9A9D}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -3252,93 +3760,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CAE7036-8C5B-4AB4-B879-95C777AB2D1D}">
-  <sheetPr>
-    <tabColor rgb="FF92D050"/>
-  </sheetPr>
-  <dimension ref="A1:A13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>298</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>